<commit_message>
added CMV and ABO/Rh examples
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-cibmtr-obs-priority-variables.xlsx
+++ b/docs/StructureDefinition-cibmtr-obs-priority-variables.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2722" uniqueCount="557">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-08-10T13:28:25-05:00</t>
+    <t>2022-08-11T16:57:48-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1214,7 +1214,7 @@
   </si>
   <si>
     <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
+CodeableConcept</t>
   </si>
   <si>
     <t>Result Value</t>
@@ -1714,6 +1714,10 @@
   </si>
   <si>
     <t>Observation.component.value[x]</t>
+  </si>
+  <si>
+    <t>Quantity
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual component result</t>
@@ -10144,16 +10148,16 @@
         <v>89</v>
       </c>
       <c r="J69" t="s" s="2">
-        <v>383</v>
+        <v>542</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N69" t="s" s="2">
         <v>387</v>
@@ -10223,7 +10227,7 @@
         <v>78</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AL69" t="s" s="2">
         <v>391</v>
@@ -10240,7 +10244,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -10266,13 +10270,13 @@
         <v>281</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="N70" t="s" s="2">
         <v>398</v>
@@ -10303,7 +10307,7 @@
         <v>146</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="Y70" t="s" s="2">
         <v>399</v>
@@ -10324,7 +10328,7 @@
         <v>78</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>76</v>
@@ -10333,7 +10337,7 @@
         <v>88</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>100</v>
@@ -10359,7 +10363,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -10443,7 +10447,7 @@
         <v>78</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>76</v>
@@ -10478,7 +10482,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -10504,10 +10508,10 @@
         <v>78</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="M72" t="s" s="2">
         <v>463</v>
@@ -10562,7 +10566,7 @@
         <v>78</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>76</v>

</xml_diff>